<commit_message>
redid experiments with corect OHE scenario
</commit_message>
<xml_diff>
--- a/results/AA6000_simulation_10MC_50exp_1batch.xlsx
+++ b/results/AA6000_simulation_10MC_50exp_1batch.xlsx
@@ -20410,11 +20410,11 @@
       </c>
       <c r="F666" t="inlineStr">
         <is>
-          <t>[21.0]</t>
+          <t>[73.5]</t>
         </is>
       </c>
       <c r="G666" t="n">
-        <v>21</v>
+        <v>73.5</v>
       </c>
       <c r="H666" t="n">
         <v>75.15333333333332</v>
@@ -20440,14 +20440,14 @@
       </c>
       <c r="F667" t="inlineStr">
         <is>
-          <t>[19.0]</t>
+          <t>[81.5]</t>
         </is>
       </c>
       <c r="G667" t="n">
-        <v>19</v>
+        <v>81.5</v>
       </c>
       <c r="H667" t="n">
-        <v>75.15333333333332</v>
+        <v>81.5</v>
       </c>
     </row>
     <row r="668">
@@ -20470,14 +20470,14 @@
       </c>
       <c r="F668" t="inlineStr">
         <is>
-          <t>[69.5]</t>
+          <t>[67.375]</t>
         </is>
       </c>
       <c r="G668" t="n">
-        <v>69.5</v>
+        <v>67.375</v>
       </c>
       <c r="H668" t="n">
-        <v>75.15333333333332</v>
+        <v>81.5</v>
       </c>
     </row>
     <row r="669">
@@ -20500,14 +20500,14 @@
       </c>
       <c r="F669" t="inlineStr">
         <is>
-          <t>[67.375]</t>
+          <t>[19.0]</t>
         </is>
       </c>
       <c r="G669" t="n">
-        <v>67.375</v>
+        <v>19</v>
       </c>
       <c r="H669" t="n">
-        <v>75.15333333333332</v>
+        <v>81.5</v>
       </c>
     </row>
     <row r="670">
@@ -20530,14 +20530,14 @@
       </c>
       <c r="F670" t="inlineStr">
         <is>
-          <t>[73.5]</t>
+          <t>[21.0]</t>
         </is>
       </c>
       <c r="G670" t="n">
-        <v>73.5</v>
+        <v>21</v>
       </c>
       <c r="H670" t="n">
-        <v>75.15333333333332</v>
+        <v>81.5</v>
       </c>
     </row>
     <row r="671">
@@ -20567,7 +20567,7 @@
         <v>75.26333333333334</v>
       </c>
       <c r="H671" t="n">
-        <v>75.26333333333334</v>
+        <v>81.5</v>
       </c>
     </row>
     <row r="672">
@@ -20590,14 +20590,14 @@
       </c>
       <c r="F672" t="inlineStr">
         <is>
-          <t>[81.5]</t>
+          <t>[85.0]</t>
         </is>
       </c>
       <c r="G672" t="n">
-        <v>81.5</v>
+        <v>85</v>
       </c>
       <c r="H672" t="n">
-        <v>81.5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="673">
@@ -20620,11 +20620,11 @@
       </c>
       <c r="F673" t="inlineStr">
         <is>
-          <t>[85.0]</t>
+          <t>[69.5]</t>
         </is>
       </c>
       <c r="G673" t="n">
-        <v>85</v>
+        <v>69.5</v>
       </c>
       <c r="H673" t="n">
         <v>85</v>
@@ -20650,11 +20650,11 @@
       </c>
       <c r="F674" t="inlineStr">
         <is>
-          <t>[81.5]</t>
+          <t>[76.625]</t>
         </is>
       </c>
       <c r="G674" t="n">
-        <v>81.5</v>
+        <v>76.625</v>
       </c>
       <c r="H674" t="n">
         <v>85</v>
@@ -20680,11 +20680,11 @@
       </c>
       <c r="F675" t="inlineStr">
         <is>
-          <t>[76.625]</t>
+          <t>[81.5]</t>
         </is>
       </c>
       <c r="G675" t="n">
-        <v>76.625</v>
+        <v>81.5</v>
       </c>
       <c r="H675" t="n">
         <v>85</v>
@@ -21130,11 +21130,11 @@
       </c>
       <c r="F690" t="inlineStr">
         <is>
-          <t>[75.15333333333332]</t>
+          <t>[75.26333333333334]</t>
         </is>
       </c>
       <c r="G690" t="n">
-        <v>75.15333333333332</v>
+        <v>75.26333333333334</v>
       </c>
       <c r="H690" t="n">
         <v>81.5</v>
@@ -21160,11 +21160,11 @@
       </c>
       <c r="F691" t="inlineStr">
         <is>
-          <t>[75.26333333333334]</t>
+          <t>[75.15333333333332]</t>
         </is>
       </c>
       <c r="G691" t="n">
-        <v>75.26333333333334</v>
+        <v>75.15333333333332</v>
       </c>
       <c r="H691" t="n">
         <v>81.5</v>
@@ -21730,11 +21730,11 @@
       </c>
       <c r="F710" t="inlineStr">
         <is>
-          <t>[21.0]</t>
+          <t>[73.5]</t>
         </is>
       </c>
       <c r="G710" t="n">
-        <v>21</v>
+        <v>73.5</v>
       </c>
       <c r="H710" t="n">
         <v>75.15333333333332</v>
@@ -21760,14 +21760,14 @@
       </c>
       <c r="F711" t="inlineStr">
         <is>
-          <t>[19.0]</t>
+          <t>[81.5]</t>
         </is>
       </c>
       <c r="G711" t="n">
-        <v>19</v>
+        <v>81.5</v>
       </c>
       <c r="H711" t="n">
-        <v>75.15333333333332</v>
+        <v>81.5</v>
       </c>
     </row>
     <row r="712">
@@ -21790,14 +21790,14 @@
       </c>
       <c r="F712" t="inlineStr">
         <is>
-          <t>[69.5]</t>
+          <t>[67.375]</t>
         </is>
       </c>
       <c r="G712" t="n">
-        <v>69.5</v>
+        <v>67.375</v>
       </c>
       <c r="H712" t="n">
-        <v>75.15333333333332</v>
+        <v>81.5</v>
       </c>
     </row>
     <row r="713">
@@ -21820,14 +21820,14 @@
       </c>
       <c r="F713" t="inlineStr">
         <is>
-          <t>[67.375]</t>
+          <t>[19.0]</t>
         </is>
       </c>
       <c r="G713" t="n">
-        <v>67.375</v>
+        <v>19</v>
       </c>
       <c r="H713" t="n">
-        <v>75.15333333333332</v>
+        <v>81.5</v>
       </c>
     </row>
     <row r="714">
@@ -21850,14 +21850,14 @@
       </c>
       <c r="F714" t="inlineStr">
         <is>
-          <t>[73.5]</t>
+          <t>[21.0]</t>
         </is>
       </c>
       <c r="G714" t="n">
-        <v>73.5</v>
+        <v>21</v>
       </c>
       <c r="H714" t="n">
-        <v>75.15333333333332</v>
+        <v>81.5</v>
       </c>
     </row>
     <row r="715">
@@ -21880,14 +21880,14 @@
       </c>
       <c r="F715" t="inlineStr">
         <is>
-          <t>[85.0]</t>
+          <t>[75.26333333333334]</t>
         </is>
       </c>
       <c r="G715" t="n">
-        <v>85</v>
+        <v>75.26333333333334</v>
       </c>
       <c r="H715" t="n">
-        <v>85</v>
+        <v>81.5</v>
       </c>
     </row>
     <row r="716">
@@ -21910,14 +21910,14 @@
       </c>
       <c r="F716" t="inlineStr">
         <is>
-          <t>[81.5]</t>
+          <t>[76.625]</t>
         </is>
       </c>
       <c r="G716" t="n">
+        <v>76.625</v>
+      </c>
+      <c r="H716" t="n">
         <v>81.5</v>
-      </c>
-      <c r="H716" t="n">
-        <v>85</v>
       </c>
     </row>
     <row r="717">
@@ -21940,14 +21940,14 @@
       </c>
       <c r="F717" t="inlineStr">
         <is>
-          <t>[76.625]</t>
+          <t>[69.5]</t>
         </is>
       </c>
       <c r="G717" t="n">
-        <v>76.625</v>
+        <v>69.5</v>
       </c>
       <c r="H717" t="n">
-        <v>85</v>
+        <v>81.5</v>
       </c>
     </row>
     <row r="718">
@@ -21970,11 +21970,11 @@
       </c>
       <c r="F718" t="inlineStr">
         <is>
-          <t>[75.26333333333334]</t>
+          <t>[85.0]</t>
         </is>
       </c>
       <c r="G718" t="n">
-        <v>75.26333333333334</v>
+        <v>85</v>
       </c>
       <c r="H718" t="n">
         <v>85</v>
@@ -22960,11 +22960,11 @@
       </c>
       <c r="F751" t="inlineStr">
         <is>
-          <t>[59.125]</t>
+          <t>[19.0]</t>
         </is>
       </c>
       <c r="G751" t="n">
-        <v>59.125</v>
+        <v>19</v>
       </c>
       <c r="H751" t="n">
         <v>73.5</v>
@@ -23050,11 +23050,11 @@
       </c>
       <c r="F754" t="inlineStr">
         <is>
-          <t>[76.625]</t>
+          <t>[59.125]</t>
         </is>
       </c>
       <c r="G754" t="n">
-        <v>76.625</v>
+        <v>59.125</v>
       </c>
       <c r="H754" t="n">
         <v>81.5</v>
@@ -23080,11 +23080,11 @@
       </c>
       <c r="F755" t="inlineStr">
         <is>
-          <t>[56.625]</t>
+          <t>[75.26333333333334]</t>
         </is>
       </c>
       <c r="G755" t="n">
-        <v>56.625</v>
+        <v>75.26333333333334</v>
       </c>
       <c r="H755" t="n">
         <v>81.5</v>
@@ -23110,11 +23110,11 @@
       </c>
       <c r="F756" t="inlineStr">
         <is>
-          <t>[19.0]</t>
+          <t>[75.15333333333332]</t>
         </is>
       </c>
       <c r="G756" t="n">
-        <v>19</v>
+        <v>75.15333333333332</v>
       </c>
       <c r="H756" t="n">
         <v>81.5</v>
@@ -23140,11 +23140,11 @@
       </c>
       <c r="F757" t="inlineStr">
         <is>
-          <t>[75.26333333333334]</t>
+          <t>[21.0]</t>
         </is>
       </c>
       <c r="G757" t="n">
-        <v>75.26333333333334</v>
+        <v>21</v>
       </c>
       <c r="H757" t="n">
         <v>81.5</v>
@@ -23170,11 +23170,11 @@
       </c>
       <c r="F758" t="inlineStr">
         <is>
-          <t>[75.15333333333332]</t>
+          <t>[56.625]</t>
         </is>
       </c>
       <c r="G758" t="n">
-        <v>75.15333333333332</v>
+        <v>56.625</v>
       </c>
       <c r="H758" t="n">
         <v>81.5</v>
@@ -23200,11 +23200,11 @@
       </c>
       <c r="F759" t="inlineStr">
         <is>
-          <t>[21.0]</t>
+          <t>[74.08666666666666]</t>
         </is>
       </c>
       <c r="G759" t="n">
-        <v>21</v>
+        <v>74.08666666666666</v>
       </c>
       <c r="H759" t="n">
         <v>81.5</v>
@@ -23230,14 +23230,14 @@
       </c>
       <c r="F760" t="inlineStr">
         <is>
-          <t>[69.5]</t>
+          <t>[85.0]</t>
         </is>
       </c>
       <c r="G760" t="n">
-        <v>69.5</v>
+        <v>85</v>
       </c>
       <c r="H760" t="n">
-        <v>81.5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="761">
@@ -23260,14 +23260,14 @@
       </c>
       <c r="F761" t="inlineStr">
         <is>
-          <t>[74.08666666666666]</t>
+          <t>[69.5]</t>
         </is>
       </c>
       <c r="G761" t="n">
-        <v>74.08666666666666</v>
+        <v>69.5</v>
       </c>
       <c r="H761" t="n">
-        <v>81.5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="762">
@@ -23290,11 +23290,11 @@
       </c>
       <c r="F762" t="inlineStr">
         <is>
-          <t>[85.0]</t>
+          <t>[76.625]</t>
         </is>
       </c>
       <c r="G762" t="n">
-        <v>85</v>
+        <v>76.625</v>
       </c>
       <c r="H762" t="n">
         <v>85</v>
@@ -24430,11 +24430,11 @@
       </c>
       <c r="F800" t="inlineStr">
         <is>
-          <t>[75.15333333333332]</t>
+          <t>[75.26333333333334]</t>
         </is>
       </c>
       <c r="G800" t="n">
-        <v>75.15333333333332</v>
+        <v>75.26333333333334</v>
       </c>
       <c r="H800" t="n">
         <v>81.5</v>
@@ -24460,11 +24460,11 @@
       </c>
       <c r="F801" t="inlineStr">
         <is>
-          <t>[75.26333333333334]</t>
+          <t>[75.15333333333332]</t>
         </is>
       </c>
       <c r="G801" t="n">
-        <v>75.26333333333334</v>
+        <v>75.15333333333332</v>
       </c>
       <c r="H801" t="n">
         <v>81.5</v>
@@ -25780,14 +25780,14 @@
       </c>
       <c r="F845" t="inlineStr">
         <is>
-          <t>[85.0]</t>
+          <t>[81.5]</t>
         </is>
       </c>
       <c r="G845" t="n">
-        <v>85</v>
+        <v>81.5</v>
       </c>
       <c r="H845" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="846">
@@ -25810,14 +25810,14 @@
       </c>
       <c r="F846" t="inlineStr">
         <is>
-          <t>[67.375]</t>
+          <t>[81.5]</t>
         </is>
       </c>
       <c r="G846" t="n">
-        <v>67.375</v>
+        <v>81.5</v>
       </c>
       <c r="H846" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="847">
@@ -25840,14 +25840,14 @@
       </c>
       <c r="F847" t="inlineStr">
         <is>
-          <t>[81.5]</t>
+          <t>[74.125]</t>
         </is>
       </c>
       <c r="G847" t="n">
-        <v>81.5</v>
+        <v>74.125</v>
       </c>
       <c r="H847" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="848">
@@ -25870,11 +25870,11 @@
       </c>
       <c r="F848" t="inlineStr">
         <is>
-          <t>[81.5]</t>
+          <t>[85.0]</t>
         </is>
       </c>
       <c r="G848" t="n">
-        <v>81.5</v>
+        <v>85</v>
       </c>
       <c r="H848" t="n">
         <v>85</v>
@@ -25900,11 +25900,11 @@
       </c>
       <c r="F849" t="inlineStr">
         <is>
-          <t>[76.625]</t>
+          <t>[21.0]</t>
         </is>
       </c>
       <c r="G849" t="n">
-        <v>76.625</v>
+        <v>21</v>
       </c>
       <c r="H849" t="n">
         <v>85</v>
@@ -25930,11 +25930,11 @@
       </c>
       <c r="F850" t="inlineStr">
         <is>
-          <t>[21.0]</t>
+          <t>[19.0]</t>
         </is>
       </c>
       <c r="G850" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H850" t="n">
         <v>85</v>
@@ -25960,11 +25960,11 @@
       </c>
       <c r="F851" t="inlineStr">
         <is>
-          <t>[19.0]</t>
+          <t>[73.5]</t>
         </is>
       </c>
       <c r="G851" t="n">
-        <v>19</v>
+        <v>73.5</v>
       </c>
       <c r="H851" t="n">
         <v>85</v>
@@ -25990,11 +25990,11 @@
       </c>
       <c r="F852" t="inlineStr">
         <is>
-          <t>[73.5]</t>
+          <t>[79.0]</t>
         </is>
       </c>
       <c r="G852" t="n">
-        <v>73.5</v>
+        <v>79</v>
       </c>
       <c r="H852" t="n">
         <v>85</v>
@@ -26020,11 +26020,11 @@
       </c>
       <c r="F853" t="inlineStr">
         <is>
-          <t>[79.0]</t>
+          <t>[75.15333333333332]</t>
         </is>
       </c>
       <c r="G853" t="n">
-        <v>79</v>
+        <v>75.15333333333332</v>
       </c>
       <c r="H853" t="n">
         <v>85</v>
@@ -26050,11 +26050,11 @@
       </c>
       <c r="F854" t="inlineStr">
         <is>
-          <t>[74.125]</t>
+          <t>[76.625]</t>
         </is>
       </c>
       <c r="G854" t="n">
-        <v>74.125</v>
+        <v>76.625</v>
       </c>
       <c r="H854" t="n">
         <v>85</v>
@@ -26080,11 +26080,11 @@
       </c>
       <c r="F855" t="inlineStr">
         <is>
-          <t>[77.0]</t>
+          <t>[67.375]</t>
         </is>
       </c>
       <c r="G855" t="n">
-        <v>77</v>
+        <v>67.375</v>
       </c>
       <c r="H855" t="n">
         <v>85</v>
@@ -26110,11 +26110,11 @@
       </c>
       <c r="F856" t="inlineStr">
         <is>
-          <t>[75.15333333333332]</t>
+          <t>[77.0]</t>
         </is>
       </c>
       <c r="G856" t="n">
-        <v>75.15333333333332</v>
+        <v>77</v>
       </c>
       <c r="H856" t="n">
         <v>85</v>

</xml_diff>